<commit_message>
Importing items is implemented.
</commit_message>
<xml_diff>
--- a/Refuntations_App/wwwroot/IMPORT - Akcijska aktivnost - PDV - SAP Kljuc - MATERIJAL - BANER.xlsx
+++ b/Refuntations_App/wwwroot/IMPORT - Akcijska aktivnost - PDV - SAP Kljuc - MATERIJAL - BANER.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dste848075\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dste848075\Desktop\Refundacije\Refuntations_App\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Sifra  INO Dobavljac</t>
+    <t>Sifra  AA</t>
   </si>
   <si>
-    <t>Naziv INO Dobavljac</t>
+    <t>Naziv AA</t>
+  </si>
+  <si>
+    <t>PDV</t>
+  </si>
+  <si>
+    <t>SAP KLJUC</t>
+  </si>
+  <si>
+    <t>MATERIJAL</t>
   </si>
 </sst>
 </file>
@@ -74,10 +83,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -360,24 +372,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="42" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>